<commit_message>
It's now possible to edit existing number cells.
</commit_message>
<xml_diff>
--- a/XLSXLibExample/Example/Testfile.xlsx
+++ b/XLSXLibExample/Example/Testfile.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damml\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF5A9A17-D555-4711-BB26-69B94BAF201A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{596E4B81-4FEC-41F3-A2C3-9C374522C223}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId3"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,9 +34,13 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,13 +48,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFE0000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF01"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,17 +104,131 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,131 +536,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44C19AE-F7F7-4FFE-AC60-AADE44B84370}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44C19AE-F7F7-4FFE-AC60-AADE44B84370}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A1" sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.424285714285714" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15">
       <c r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5139763-C99C-4B3B-BE24-C6BA419CC2D3}">
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5139763-C99C-4B3B-BE24-C6BA419CC2D3}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.424285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="11.428571428571429" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:1" ht="15" customHeight="1">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:1" ht="15" customHeight="1">
+      <c r="A2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:1" ht="15" customHeight="1">
+      <c r="A3" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:1" ht="15">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>